<commit_message>
Fix: Photosynthesis issue was resolved
</commit_message>
<xml_diff>
--- a/v3-0-OOP-operational/Default_Inputs.xlsx
+++ b/v3-0-OOP-operational/Default_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diane_lab\simple_model\generic_crop_model_project\Git_OOD\Generic-Object-Oriented-Plant-Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diane_lab\simple_model\generic_crop_model_project\Git_OOD\Generic-Object-Oriented-Plant-Model\v3-0-OOP-operational\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CBC352-FF2A-4EE6-BDAF-FE8F87EF8B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040D5A51-9AA7-43A2-8B48-204CFF7A3666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{572359C2-A4E8-42F8-B0B6-79384554FF68}"/>
   </bookViews>
@@ -544,8 +544,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -590,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>0.05</v>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -614,7 +614,7 @@
         <v>33</v>
       </c>
       <c r="B8">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>